<commit_message>
Updated metrics value and added new script - updated metrics and predictions by put zero on negative predictions on salinity and ck - added script to run lx prediction on 2016 - 2019  dataset for hybrid model implmentation
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Ck_Parameters_Estimation/1-Trained-Models/training_test_2016_2019_new_cal/pwbTable.xlsx
+++ b/Parameters-Estimation/Ck_Parameters_Estimation/1-Trained-Models/training_test_2016_2019_new_cal/pwbTable.xlsx
@@ -13,24 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Row</t>
-  </si>
-  <si>
-    <t>PWB1</t>
-  </si>
-  <si>
-    <t>PWB5</t>
-  </si>
-  <si>
-    <t>PWB10</t>
-  </si>
-  <si>
-    <t>PWB20</t>
-  </si>
-  <si>
-    <t>PWB30</t>
+    <t>EBM</t>
   </si>
   <si>
     <t>random_forest</t>
@@ -40,9 +25,6 @@
   </si>
   <si>
     <t>neural_network</t>
-  </si>
-  <si>
-    <t>EBM</t>
   </si>
 </sst>
 </file>
@@ -88,14 +70,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" customWidth="true"/>
+    <col min="1" max="1" width="5.7109375" customWidth="true"/>
     <col min="2" max="2" width="14.28515625" customWidth="true"/>
     <col min="3" max="3" width="7.5703125" customWidth="true"/>
     <col min="4" max="4" width="15.28515625" customWidth="true"/>
-    <col min="5" max="5" width="5.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -103,101 +84,83 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
+      <c r="A2" s="0">
+        <v>1.6799999999999999</v>
       </c>
       <c r="B2" s="0">
         <v>2.9399999999999999</v>
       </c>
       <c r="C2" s="0">
-        <v>1.26</v>
+        <v>2.1000000000000001</v>
       </c>
       <c r="D2" s="0">
-        <v>2.1000000000000001</v>
-      </c>
-      <c r="E2" s="0">
-        <v>1.6799999999999999</v>
+        <v>3.7799999999999998</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
+      <c r="A3" s="0">
+        <v>8.8200000000000003</v>
       </c>
       <c r="B3" s="0">
         <v>11.34</v>
       </c>
       <c r="C3" s="0">
-        <v>8.8200000000000003</v>
+        <v>9.6600000000000001</v>
       </c>
       <c r="D3" s="0">
-        <v>7.9800000000000004</v>
-      </c>
-      <c r="E3" s="0">
-        <v>8.8200000000000003</v>
+        <v>9.6600000000000001</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
+      <c r="A4" s="0">
+        <v>18.91</v>
       </c>
       <c r="B4" s="0">
         <v>21.850000000000001</v>
       </c>
       <c r="C4" s="0">
-        <v>19.329999999999998</v>
+        <v>20.170000000000002</v>
       </c>
       <c r="D4" s="0">
-        <v>21.010000000000002</v>
-      </c>
-      <c r="E4" s="0">
-        <v>18.91</v>
+        <v>22.690000000000001</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>4</v>
+      <c r="A5" s="0">
+        <v>34.450000000000003</v>
       </c>
       <c r="B5" s="0">
         <v>39.5</v>
       </c>
       <c r="C5" s="0">
-        <v>41.600000000000001</v>
+        <v>42.439999999999998</v>
       </c>
       <c r="D5" s="0">
-        <v>42.020000000000003</v>
-      </c>
-      <c r="E5" s="0">
-        <v>34.450000000000003</v>
+        <v>43.700000000000003</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>5</v>
+      <c r="A6" s="0">
+        <v>47.899999999999999</v>
       </c>
       <c r="B6" s="0">
         <v>57.560000000000002</v>
       </c>
       <c r="C6" s="0">
-        <v>56.299999999999997</v>
+        <v>57.140000000000001</v>
       </c>
       <c r="D6" s="0">
-        <v>55.039999999999999</v>
-      </c>
-      <c r="E6" s="0">
-        <v>47.899999999999999</v>
+        <v>56.719999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>